<commit_message>
finishing model, has errors
</commit_message>
<xml_diff>
--- a/Dow 30/Goldman/Goldman.xlsx
+++ b/Dow 30/Goldman/Goldman.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\Dow Valuation\Dow 30\Goldman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1DE293-DAEA-4276-8050-F30427DFA707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF751B-3DE3-46A4-BB60-9A147CDCDC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{A3E34BEC-3060-4EA5-9DCA-0D4090F72745}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{A3E34BEC-3060-4EA5-9DCA-0D4090F72745}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical Data and Projections" sheetId="1" r:id="rId1"/>
     <sheet name="Street Estimates" sheetId="2" r:id="rId2"/>
+    <sheet name="DCF Model" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
   <si>
     <t>Ticker: GS</t>
   </si>
@@ -186,17 +187,130 @@
   </si>
   <si>
     <t>NWC:</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>Growth Rate</t>
+  </si>
+  <si>
+    <t>EV / EBITDA</t>
+  </si>
+  <si>
+    <t>Cost of Debt</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Risk Free Rate</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Market Return</t>
+  </si>
+  <si>
+    <t>Debt Value</t>
+  </si>
+  <si>
+    <t>Equity Value</t>
+  </si>
+  <si>
+    <t>WACC:</t>
+  </si>
+  <si>
+    <t>FCF</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>EBIT</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>D&amp;A</t>
+  </si>
+  <si>
+    <t>NWC</t>
+  </si>
+  <si>
+    <t>Cost of Equity</t>
+  </si>
+  <si>
+    <t>D/D+E</t>
+  </si>
+  <si>
+    <t>E/D+E</t>
+  </si>
+  <si>
+    <t>WACC</t>
+  </si>
+  <si>
+    <t>Terminal Value</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>Perpetuity Growth</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Discounting</t>
+  </si>
+  <si>
+    <t>Discount Factor</t>
+  </si>
+  <si>
+    <t>PV of FCF</t>
+  </si>
+  <si>
+    <t>PV of TV</t>
+  </si>
+  <si>
+    <t>Enterprise Value</t>
+  </si>
+  <si>
+    <t>Enterprise Value to Equity Value</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Marketable Securities</t>
+  </si>
+  <si>
+    <t>Long-term Debt</t>
+  </si>
+  <si>
+    <t>Short-term Debt</t>
+  </si>
+  <si>
+    <t>Shares Outstanding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\(#,##0\)_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\(#,##0.00\)_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +329,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -356,10 +477,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -409,6 +531,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,10 +550,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1404,6 +1553,376 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Goldman Net Income to Shareholders</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Historical Data and Projections'!$E$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Historical Data and Projections'!$E$28:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\(#,##0\)_-;_-* "-"_-;_-@_-</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10459</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8466</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9459</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BFE-4CED-9B2F-A4BAC0D2D0B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1376890992"/>
+        <c:axId val="1876211056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1376890992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1876211056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1876211056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_-* #,##0_-;\(#,##0\)_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1376890992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1484,6 +2003,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1988,6 +2547,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2559,6 +3621,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A83B8F-6C88-3F7A-B5DB-62638207F32B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2866,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002A1BE5-3274-4D75-A10D-F4A6E7BE869D}">
   <dimension ref="B2:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2890,20 +3988,20 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="49" t="s">
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E4" s="5"/>
@@ -3973,19 +5071,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAC15C-87F3-4E14-AAD1-7E05F30C7757}">
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3994,28 +5099,28 @@
       <c r="E2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="49" t="s">
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E4" s="5"/>
       <c r="J4" s="5">
         <v>1</v>
@@ -4033,12 +5138,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="6">
         <v>2017</v>
       </c>
@@ -4070,164 +5175,310 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="18">
+        <v>27044</v>
+      </c>
+      <c r="J6" s="53"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="J7" s="5">
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="17">
         <v>17805</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="18">
         <v>19869</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="18">
         <v>21699</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="18">
         <v>19969</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="18">
         <v>20653</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="J8" s="5">
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="17">
         <v>17259</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="18">
         <v>17983</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="18">
         <v>20349</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="18">
         <v>19969</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="18">
         <v>20653</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="J9" s="5">
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="17">
         <v>15217</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="18">
         <v>16486</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="18">
         <v>17940</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="18">
         <v>19969</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="18">
         <v>20653</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E10" s="42">
+        <v>6846</v>
+      </c>
+      <c r="F10" s="43">
+        <v>2022</v>
+      </c>
+      <c r="G10" s="43">
+        <v>2117</v>
+      </c>
+      <c r="H10" s="43">
+        <v>3020</v>
+      </c>
+      <c r="I10" s="43">
+        <v>5409</v>
+      </c>
+      <c r="J10" s="51">
+        <f>22%*J8</f>
+        <v>3796.98</v>
+      </c>
+      <c r="K10" s="52">
+        <f>22%*K8</f>
+        <v>3956.26</v>
+      </c>
+      <c r="L10" s="52">
+        <f t="shared" ref="L10:N10" si="0">22%*L8</f>
+        <v>4476.78</v>
+      </c>
+      <c r="M10" s="52">
+        <f t="shared" si="0"/>
+        <v>4393.18</v>
+      </c>
+      <c r="N10" s="52">
+        <f t="shared" si="0"/>
+        <v>4543.66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E11" s="42">
+        <v>1152</v>
+      </c>
+      <c r="F11" s="43">
+        <v>1328</v>
+      </c>
+      <c r="G11" s="43">
+        <v>1704</v>
+      </c>
+      <c r="H11" s="43">
+        <v>1902</v>
+      </c>
+      <c r="I11" s="43">
+        <v>2015</v>
+      </c>
+      <c r="J11" s="42">
+        <v>1920</v>
+      </c>
+      <c r="K11" s="52">
+        <f>1.01*J11</f>
+        <v>1939.2</v>
+      </c>
+      <c r="L11" s="52">
+        <f t="shared" ref="L11:N11" si="1">1.01*K11</f>
+        <v>1958.5920000000001</v>
+      </c>
+      <c r="M11" s="52">
+        <f t="shared" si="1"/>
+        <v>1978.1779200000001</v>
+      </c>
+      <c r="N11" s="52">
+        <f t="shared" si="1"/>
+        <v>1997.9596992000002</v>
+      </c>
+      <c r="P11" s="50"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E12" s="26">
+        <v>3184</v>
+      </c>
+      <c r="F12" s="27">
+        <v>7982</v>
+      </c>
+      <c r="G12" s="27">
+        <v>8443</v>
+      </c>
+      <c r="H12" s="27">
+        <v>6309</v>
+      </c>
+      <c r="I12" s="27">
+        <v>4667</v>
+      </c>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="53">
+        <f>1.387*I12</f>
+        <v>6473.1289999999999</v>
+      </c>
+      <c r="K14" s="54">
+        <f>1.05*J14</f>
+        <v>6796.7854500000003</v>
+      </c>
+      <c r="L14" s="54">
+        <f>1.029*K14</f>
+        <v>6993.8922280500001</v>
+      </c>
+      <c r="M14" s="54">
+        <f>1.001*L14</f>
+        <v>7000.886120278049</v>
+      </c>
+      <c r="N14" s="54">
+        <f>1.034*M14</f>
+        <v>7238.9162483675027</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="E16" s="42">
+        <v>-108700</v>
+      </c>
+      <c r="F16" s="43">
+        <v>-38971</v>
+      </c>
+      <c r="G16" s="43">
+        <v>-2096</v>
+      </c>
+      <c r="H16" s="43">
+        <v>8533</v>
+      </c>
+      <c r="I16" s="43">
+        <v>-87129</v>
+      </c>
+      <c r="J16" s="51">
+        <f>-0.197*I16+I16</f>
+        <v>-69964.587</v>
+      </c>
+      <c r="K16" s="52">
+        <f>1.05*J16</f>
+        <v>-73462.816350000008</v>
+      </c>
+      <c r="L16" s="52">
+        <f t="shared" ref="L16:N16" si="2">1.05*K16</f>
+        <v>-77135.957167500019</v>
+      </c>
+      <c r="M16" s="52">
+        <f t="shared" si="2"/>
+        <v>-80992.755025875027</v>
+      </c>
+      <c r="N16" s="52">
+        <f t="shared" si="2"/>
+        <v>-85042.392777168789</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4236,4 +5487,597 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F400E3-9F48-4E46-8AFE-5EFCB118D169}">
+  <dimension ref="B2:O45"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="I5" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="57">
+        <v>0</v>
+      </c>
+      <c r="K5" s="58">
+        <v>1</v>
+      </c>
+      <c r="L5" s="58">
+        <v>2</v>
+      </c>
+      <c r="M5" s="58">
+        <v>3</v>
+      </c>
+      <c r="N5" s="58">
+        <v>4</v>
+      </c>
+      <c r="O5" s="58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="53">
+        <f>'Street Estimates'!I6</f>
+        <v>27044</v>
+      </c>
+      <c r="K6" s="54">
+        <f>'Street Estimates'!J8</f>
+        <v>17259</v>
+      </c>
+      <c r="L6" s="54">
+        <f>'Street Estimates'!K8</f>
+        <v>17983</v>
+      </c>
+      <c r="M6" s="54">
+        <f>'Street Estimates'!L8</f>
+        <v>20349</v>
+      </c>
+      <c r="N6" s="54">
+        <f>'Street Estimates'!M8</f>
+        <v>19969</v>
+      </c>
+      <c r="O6" s="54">
+        <f>'Street Estimates'!N8</f>
+        <v>20653</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="53">
+        <f>-'Street Estimates'!I10</f>
+        <v>-5409</v>
+      </c>
+      <c r="K7" s="54">
+        <f>-'Street Estimates'!J10</f>
+        <v>-3796.98</v>
+      </c>
+      <c r="L7" s="54">
+        <f>-'Street Estimates'!K10</f>
+        <v>-3956.26</v>
+      </c>
+      <c r="M7" s="54">
+        <f>-'Street Estimates'!L10</f>
+        <v>-4476.78</v>
+      </c>
+      <c r="N7" s="54">
+        <f>-'Street Estimates'!M10</f>
+        <v>-4393.18</v>
+      </c>
+      <c r="O7" s="54">
+        <f>-'Street Estimates'!N10</f>
+        <v>-4543.66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="73">
+        <v>-0.02</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="53">
+        <f>'Street Estimates'!I11</f>
+        <v>2015</v>
+      </c>
+      <c r="K8" s="54">
+        <f>'Street Estimates'!J11</f>
+        <v>1920</v>
+      </c>
+      <c r="L8" s="54">
+        <f>'Street Estimates'!K11</f>
+        <v>1939.2</v>
+      </c>
+      <c r="M8" s="54">
+        <f>'Street Estimates'!L11</f>
+        <v>1958.5920000000001</v>
+      </c>
+      <c r="N8" s="54">
+        <f>'Street Estimates'!M11</f>
+        <v>1978.1779200000001</v>
+      </c>
+      <c r="O8" s="54">
+        <f>'Street Estimates'!N11</f>
+        <v>1997.9596992000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="20">
+        <v>27.93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="53">
+        <f>-'Street Estimates'!I12</f>
+        <v>-4667</v>
+      </c>
+      <c r="K9" s="54">
+        <f>-'Street Estimates'!J14</f>
+        <v>-6473.1289999999999</v>
+      </c>
+      <c r="L9" s="54">
+        <f>-'Street Estimates'!K14</f>
+        <v>-6796.7854500000003</v>
+      </c>
+      <c r="M9" s="54">
+        <f>-'Street Estimates'!L14</f>
+        <v>-6993.8922280500001</v>
+      </c>
+      <c r="N9" s="54">
+        <f>-'Street Estimates'!M14</f>
+        <v>-7000.886120278049</v>
+      </c>
+      <c r="O9" s="54">
+        <f>-'Street Estimates'!N14</f>
+        <v>-7238.9162483675027</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="73">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="53">
+        <f>-'Street Estimates'!I16</f>
+        <v>87129</v>
+      </c>
+      <c r="K10" s="54">
+        <f>-'Street Estimates'!J16</f>
+        <v>69964.587</v>
+      </c>
+      <c r="L10" s="54">
+        <f>-'Street Estimates'!K16</f>
+        <v>73462.816350000008</v>
+      </c>
+      <c r="M10" s="54">
+        <f>-'Street Estimates'!L16</f>
+        <v>77135.957167500019</v>
+      </c>
+      <c r="N10" s="54">
+        <f>-'Street Estimates'!M16</f>
+        <v>80992.755025875027</v>
+      </c>
+      <c r="O10" s="54">
+        <f>-'Street Estimates'!N16</f>
+        <v>85042.392777168789</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="74">
+        <v>0.22</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="55">
+        <f>SUM(J6:J10)</f>
+        <v>106112</v>
+      </c>
+      <c r="K11" s="56">
+        <f>SUM(K6:K10)</f>
+        <v>78873.478000000003</v>
+      </c>
+      <c r="L11" s="56">
+        <f t="shared" ref="L11:O11" si="0">SUM(L6:L10)</f>
+        <v>82631.970900000015</v>
+      </c>
+      <c r="M11" s="56">
+        <f t="shared" si="0"/>
+        <v>87972.876939450012</v>
+      </c>
+      <c r="N11" s="56">
+        <f t="shared" si="0"/>
+        <v>91545.866825596982</v>
+      </c>
+      <c r="O11" s="56">
+        <f t="shared" si="0"/>
+        <v>95910.776228001283</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="73">
+        <v>2.7900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="20">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="75">
+        <v>99233</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="75">
+        <v>586200</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="63">
+        <f>G12+G14*(G15-G12)</f>
+        <v>8.6418999999999996E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="64">
+        <f>G17/SUM(G16:G17)</f>
+        <v>0.85522582075855702</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="64">
+        <f>G16/SUM(G16:G17)</f>
+        <v>0.14477417924144301</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="67">
+        <f>G22*G20+G21*G10*(1-G11)</f>
+        <v>4.3196742244683291E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="54">
+        <f>O6+O8</f>
+        <v>22650.959699200001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="54">
+        <f>G26*G9</f>
+        <v>632641.30439865601</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="70">
+        <f>O11*(1+G8)/(G23-G8)</f>
+        <v>1487300.7272989424</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="54">
+        <f>AVERAGE(G27:G28)</f>
+        <v>1059971.0158487991</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G30" s="54"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49">
+        <v>1</v>
+      </c>
+      <c r="H31" s="49">
+        <v>2</v>
+      </c>
+      <c r="I31" s="49">
+        <v>3</v>
+      </c>
+      <c r="J31" s="49">
+        <v>4</v>
+      </c>
+      <c r="K31" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="69">
+        <f>1/(1+$G$23)^K5</f>
+        <v>0.95859195059243063</v>
+      </c>
+      <c r="H32" s="69">
+        <f t="shared" ref="H32:K32" si="1">1/(1+$G$23)^L5</f>
+        <v>0.91889852774060088</v>
+      </c>
+      <c r="I32" s="69">
+        <f t="shared" si="1"/>
+        <v>0.88084873210337533</v>
+      </c>
+      <c r="J32" s="69">
+        <f t="shared" si="1"/>
+        <v>0.84437450428384386</v>
+      </c>
+      <c r="K32" s="69">
+        <f t="shared" si="1"/>
+        <v>0.80941060309196666</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="54">
+        <f>K11*G32</f>
+        <v>75607.481126029161</v>
+      </c>
+      <c r="H33" s="54">
+        <f t="shared" ref="H33:K33" si="2">L11*H32</f>
+        <v>75930.39640431419</v>
+      </c>
+      <c r="I33" s="54">
+        <f t="shared" si="2"/>
+        <v>77490.797111600812</v>
+      </c>
+      <c r="J33" s="54">
+        <f t="shared" si="2"/>
+        <v>77298.995920098241</v>
+      </c>
+      <c r="K33" s="54">
+        <f t="shared" si="2"/>
+        <v>77631.199229725171</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54">
+        <f>K32*G29</f>
+        <v>857951.77919818112</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="54">
+        <f>SUM(G33:K34)</f>
+        <v>1241910.6489899487</v>
+      </c>
+      <c r="H35" s="54"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="75">
+        <v>1040000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="75">
+        <v>302300</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="76">
+        <v>263500</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="72">
+        <f>F35+F38-F40-F41</f>
+        <v>1716110.6489899484</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="76">
+        <v>325420</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="68">
+        <f>F42/F44</f>
+        <v>5.2735254409377061</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>